<commit_message>
add reference controls to cyfun2025
fix SAIF excel
Improve display of reference controls when name empty
</commit_message>
<xml_diff>
--- a/tools/excel/google/google-saif_new.xlsx
+++ b/tools/excel/google/google-saif_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/excel/google/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB85568-CB68-9944-A095-4E58E5A2058C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1B74AF-97E7-B54A-800E-E8A0A6ECFD38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20400" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20400" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="189">
   <si>
     <t>type</t>
   </si>
@@ -446,9 +446,6 @@
     <t>CR</t>
   </si>
   <si>
-    <t>1:GSC-10</t>
-  </si>
-  <si>
     <t>1:UTD,1:ISD</t>
   </si>
   <si>
@@ -458,9 +455,6 @@
     <t>Are you able to detect, remove, and remediate malicious or accidental changes in your training, tuning, or evaluation data?</t>
   </si>
   <si>
-    <t>1:GSC-11,1:GSC-20,1:GSC-21,1:GSC-22,1:GSC-23</t>
-  </si>
-  <si>
     <t>1:DP</t>
   </si>
   <si>
@@ -470,9 +464,6 @@
     <t>Is any sensitive user data used in training, tuning, or evaluating your AI models?</t>
   </si>
   <si>
-    <t>1:GSC-09,1:GSC-12,1:GSC-19</t>
-  </si>
-  <si>
     <t>1:SDD</t>
   </si>
   <si>
@@ -485,9 +476,6 @@
     <t>CR,CO</t>
   </si>
   <si>
-    <t>1:GSC-12</t>
-  </si>
-  <si>
     <t>1:EDH,1:SDD</t>
   </si>
   <si>
@@ -497,9 +485,6 @@
     <t>Do you have a complete inventory of all models, datasets (for training, tuning, or evaluation), and related ML artifacts (such as code)?</t>
   </si>
   <si>
-    <t>1:GSC-20</t>
-  </si>
-  <si>
     <t>1:DP,1:MST,1:MXF</t>
   </si>
   <si>
@@ -509,18 +494,12 @@
     <t>Do you have robust access controls on all models, datasets, and related ML artifacts to minimize, detect, and prevent unauthorized reading or copying?</t>
   </si>
   <si>
-    <t>1:GSC-21</t>
-  </si>
-  <si>
     <t>2.7</t>
   </si>
   <si>
     <t>Are you able to ensure that all data, models, and code used to train, tune, or evaluate models cannot be tampered without detection during model development and during deployment?</t>
   </si>
   <si>
-    <t>1:GSC-22</t>
-  </si>
-  <si>
     <t>1:DP,1:MST</t>
   </si>
   <si>
@@ -530,9 +509,6 @@
     <t>Are the frameworks, libraries, software systems, and hardware components used in the development and deployment of your models analyzed for and protected against security vulnerabilities?</t>
   </si>
   <si>
-    <t>1:GSC-23</t>
-  </si>
-  <si>
     <t>1:DP,1:MST,1:MXF,1:MDT</t>
   </si>
   <si>
@@ -542,9 +518,6 @@
     <t>Do you protect your Generative AI applications and models against large-scale malicious queries from user accounts, devices, or via APIs?</t>
   </si>
   <si>
-    <t>1:GSC-03</t>
-  </si>
-  <si>
     <t>1:DMS,1:MRE</t>
   </si>
   <si>
@@ -563,9 +536,6 @@
     <t>Do you perform adversarial testing and training on models and Generative AI applications to improve resistance to adversarial inputs?</t>
   </si>
   <si>
-    <t>1:GSC-19,1:GSC-17</t>
-  </si>
-  <si>
     <t>1:PIJ,1:MEV,1:SDD,1:ISD,1:IMO</t>
   </si>
   <si>
@@ -575,9 +545,6 @@
     <t>Do you build or deploy Generative AI powered agents or tools that can take actions on behalf of internal or external users?</t>
   </si>
   <si>
-    <t>1:GSC-18,1:GSC-03,1:GSC-01</t>
-  </si>
-  <si>
     <t>1:PIJ,1:RA</t>
   </si>
   <si>
@@ -597,6 +564,39 @@
   </si>
   <si>
     <t>prefix_value</t>
+  </si>
+  <si>
+    <t>2:GSC-10</t>
+  </si>
+  <si>
+    <t>2:GSC-11,2:GSC-20,2:GSC-21,2:GSC-22,2:GSC-23</t>
+  </si>
+  <si>
+    <t>2:GSC-09,2:GSC-12,2:GSC-19</t>
+  </si>
+  <si>
+    <t>2:GSC-12</t>
+  </si>
+  <si>
+    <t>2:GSC-20</t>
+  </si>
+  <si>
+    <t>2:GSC-21</t>
+  </si>
+  <si>
+    <t>2:GSC-22</t>
+  </si>
+  <si>
+    <t>2:GSC-23</t>
+  </si>
+  <si>
+    <t>2:GSC-03</t>
+  </si>
+  <si>
+    <t>2:GSC-19,2:GSC-17</t>
+  </si>
+  <si>
+    <t>2:GSC-18,2:GSC-03,2:GSC-01</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1105,23 +1105,23 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScale="185" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1130,6 +1130,14 @@
       </c>
       <c r="B2" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1141,7 +1149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="161" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1173,7 +1181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="163" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -1529,7 +1537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" zoomScale="186" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1783,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="156" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1839,10 +1849,10 @@
         <v>137</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -1853,19 +1863,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>137</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1876,19 +1886,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>137</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43" x14ac:dyDescent="0.2">
@@ -1899,19 +1909,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -1922,19 +1932,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -1945,19 +1955,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43" x14ac:dyDescent="0.2">
@@ -1968,19 +1978,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>137</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43" x14ac:dyDescent="0.2">
@@ -1991,19 +2001,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>137</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -2014,19 +2024,19 @@
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -2037,19 +2047,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -2060,19 +2070,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -2083,19 +2093,19 @@
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2169,15 +2179,15 @@
         <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(lib): add reference controls in CyFun2025 (#3389)
* feat(pro): user can choose a strategy for conflicts during the import

* add reference controls to cyfun2025

fix SAIF excel
Improve display of reference controls when name empty

* Update ModelTable.svelte

fix breadcrumb

* show annotation in reference control

* prettier

* Update views.py

* add name for controls

* Add generated names for controls

Having names for controls make things much clearer.

* Update startup-tests.yml

try patch for test flakiness

---------

Co-authored-by: Abderrahmane Smimite <smimite@gmail.com>
</commit_message>
<xml_diff>
--- a/tools/excel/google/google-saif_new.xlsx
+++ b/tools/excel/google/google-saif_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/excel/google/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB85568-CB68-9944-A095-4E58E5A2058C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1B74AF-97E7-B54A-800E-E8A0A6ECFD38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20400" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20400" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="189">
   <si>
     <t>type</t>
   </si>
@@ -446,9 +446,6 @@
     <t>CR</t>
   </si>
   <si>
-    <t>1:GSC-10</t>
-  </si>
-  <si>
     <t>1:UTD,1:ISD</t>
   </si>
   <si>
@@ -458,9 +455,6 @@
     <t>Are you able to detect, remove, and remediate malicious or accidental changes in your training, tuning, or evaluation data?</t>
   </si>
   <si>
-    <t>1:GSC-11,1:GSC-20,1:GSC-21,1:GSC-22,1:GSC-23</t>
-  </si>
-  <si>
     <t>1:DP</t>
   </si>
   <si>
@@ -470,9 +464,6 @@
     <t>Is any sensitive user data used in training, tuning, or evaluating your AI models?</t>
   </si>
   <si>
-    <t>1:GSC-09,1:GSC-12,1:GSC-19</t>
-  </si>
-  <si>
     <t>1:SDD</t>
   </si>
   <si>
@@ -485,9 +476,6 @@
     <t>CR,CO</t>
   </si>
   <si>
-    <t>1:GSC-12</t>
-  </si>
-  <si>
     <t>1:EDH,1:SDD</t>
   </si>
   <si>
@@ -497,9 +485,6 @@
     <t>Do you have a complete inventory of all models, datasets (for training, tuning, or evaluation), and related ML artifacts (such as code)?</t>
   </si>
   <si>
-    <t>1:GSC-20</t>
-  </si>
-  <si>
     <t>1:DP,1:MST,1:MXF</t>
   </si>
   <si>
@@ -509,18 +494,12 @@
     <t>Do you have robust access controls on all models, datasets, and related ML artifacts to minimize, detect, and prevent unauthorized reading or copying?</t>
   </si>
   <si>
-    <t>1:GSC-21</t>
-  </si>
-  <si>
     <t>2.7</t>
   </si>
   <si>
     <t>Are you able to ensure that all data, models, and code used to train, tune, or evaluate models cannot be tampered without detection during model development and during deployment?</t>
   </si>
   <si>
-    <t>1:GSC-22</t>
-  </si>
-  <si>
     <t>1:DP,1:MST</t>
   </si>
   <si>
@@ -530,9 +509,6 @@
     <t>Are the frameworks, libraries, software systems, and hardware components used in the development and deployment of your models analyzed for and protected against security vulnerabilities?</t>
   </si>
   <si>
-    <t>1:GSC-23</t>
-  </si>
-  <si>
     <t>1:DP,1:MST,1:MXF,1:MDT</t>
   </si>
   <si>
@@ -542,9 +518,6 @@
     <t>Do you protect your Generative AI applications and models against large-scale malicious queries from user accounts, devices, or via APIs?</t>
   </si>
   <si>
-    <t>1:GSC-03</t>
-  </si>
-  <si>
     <t>1:DMS,1:MRE</t>
   </si>
   <si>
@@ -563,9 +536,6 @@
     <t>Do you perform adversarial testing and training on models and Generative AI applications to improve resistance to adversarial inputs?</t>
   </si>
   <si>
-    <t>1:GSC-19,1:GSC-17</t>
-  </si>
-  <si>
     <t>1:PIJ,1:MEV,1:SDD,1:ISD,1:IMO</t>
   </si>
   <si>
@@ -575,9 +545,6 @@
     <t>Do you build or deploy Generative AI powered agents or tools that can take actions on behalf of internal or external users?</t>
   </si>
   <si>
-    <t>1:GSC-18,1:GSC-03,1:GSC-01</t>
-  </si>
-  <si>
     <t>1:PIJ,1:RA</t>
   </si>
   <si>
@@ -597,6 +564,39 @@
   </si>
   <si>
     <t>prefix_value</t>
+  </si>
+  <si>
+    <t>2:GSC-10</t>
+  </si>
+  <si>
+    <t>2:GSC-11,2:GSC-20,2:GSC-21,2:GSC-22,2:GSC-23</t>
+  </si>
+  <si>
+    <t>2:GSC-09,2:GSC-12,2:GSC-19</t>
+  </si>
+  <si>
+    <t>2:GSC-12</t>
+  </si>
+  <si>
+    <t>2:GSC-20</t>
+  </si>
+  <si>
+    <t>2:GSC-21</t>
+  </si>
+  <si>
+    <t>2:GSC-22</t>
+  </si>
+  <si>
+    <t>2:GSC-23</t>
+  </si>
+  <si>
+    <t>2:GSC-03</t>
+  </si>
+  <si>
+    <t>2:GSC-19,2:GSC-17</t>
+  </si>
+  <si>
+    <t>2:GSC-18,2:GSC-03,2:GSC-01</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1105,23 +1105,23 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScale="185" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1130,6 +1130,14 @@
       </c>
       <c r="B2" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1141,7 +1149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="161" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1173,7 +1181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="163" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -1529,7 +1537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" zoomScale="186" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1783,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="156" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1839,10 +1849,10 @@
         <v>137</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -1853,19 +1863,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>137</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1876,19 +1886,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>137</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43" x14ac:dyDescent="0.2">
@@ -1899,19 +1909,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -1922,19 +1932,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -1945,19 +1955,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43" x14ac:dyDescent="0.2">
@@ -1968,19 +1978,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>137</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43" x14ac:dyDescent="0.2">
@@ -1991,19 +2001,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>137</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -2014,19 +2024,19 @@
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -2037,19 +2047,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -2060,19 +2070,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.2">
@@ -2083,19 +2093,19 @@
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2169,15 +2179,15 @@
         <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>